<commit_message>
Update wrapper element for MODS
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED08E392-5EA1-4951-B6A0-3D7A0E74BC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7E37D5-2C5E-4F38-A006-C2099EA563C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
+    <workbookView xWindow="1755" yWindow="555" windowWidth="25845" windowHeight="13845" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>&lt;object pid="</t>
   </si>
   <si>
-    <t>"&gt;&lt;update type="MODS"&gt;&lt;mods:mods xmlns:mods="http://www.loc.gov/mods/v3" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;</t>
-  </si>
-  <si>
     <t>&lt;mods:name type="personal"&gt;&lt;mods:namePart&gt;</t>
   </si>
   <si>
@@ -197,13 +194,16 @@
     <t>Locations</t>
   </si>
   <si>
-    <t>&lt;/mods:mods&gt;&lt;/update&gt;&lt;/object&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;mods:description&gt;Ethnic or Racial Identity: </t>
   </si>
   <si>
     <t>Ethnic or Racial Identity</t>
+  </si>
+  <si>
+    <t>"&gt;&lt;datastream type="md_descriptive" operation="update"&gt;&lt;mods:mods xmlns:mods="http://www.loc.gov/mods/v3" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/mods:mods&gt;&lt;/datastream&gt;&lt;/object&gt;</t>
   </si>
 </sst>
 </file>
@@ -577,28 +577,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
   <dimension ref="A1:BM1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BM1" sqref="BM1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" customWidth="1"/>
-    <col min="20" max="20" width="24.88671875" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" customWidth="1"/>
-    <col min="27" max="27" width="18.5546875" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" customWidth="1"/>
-    <col min="36" max="36" width="17.5546875" customWidth="1"/>
-    <col min="39" max="39" width="30.88671875" customWidth="1"/>
-    <col min="51" max="51" width="12.5546875" style="5" customWidth="1"/>
-    <col min="57" max="57" width="18.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="24.85546875" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" customWidth="1"/>
+    <col min="27" max="27" width="18.5703125" customWidth="1"/>
+    <col min="33" max="33" width="11.28515625" customWidth="1"/>
+    <col min="36" max="36" width="17.5703125" customWidth="1"/>
+    <col min="39" max="39" width="30.85546875" customWidth="1"/>
+    <col min="51" max="51" width="12.5703125" style="5" customWidth="1"/>
+    <col min="57" max="57" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -606,193 +606,193 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
         <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="R1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
         <v>26</v>
-      </c>
-      <c r="W1" t="s">
-        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Y1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
         <v>30</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>31</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AE1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" t="s">
         <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>33</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
         <v>34</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>35</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR1" t="s">
         <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>37</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AT1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU1" t="s">
         <v>38</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>39</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AW1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AX1" t="s">
         <v>40</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>41</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="AZ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA1" t="s">
         <v>42</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>43</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="BC1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BD1" t="s">
         <v>44</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>45</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="BF1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG1" t="s">
         <v>46</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>47</v>
       </c>
       <c r="BH1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="BI1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BJ1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="BK1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="BL1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BM1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SA license default
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Downloads\SA-updates-20220207\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFE3901-8CF3-42FA-AAF3-ADFD1FA1AF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96006D6A-0EE2-40AB-9B61-D08C696F0DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="1080" windowWidth="25710" windowHeight="13200" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
+    <workbookView xWindow="1200" yWindow="810" windowWidth="25710" windowHeight="13620" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -240,9 +240,6 @@
     <t>"&gt;&lt;datastream type="md_descriptive" operation="update"&gt;&lt;mods:mods xmlns:mods="http://www.loc.gov/mods/v3" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;</t>
   </si>
   <si>
-    <t>&lt;mods:accessCondition displayLabel="License" type="use and reproduction" xlink:href="https://creativecommons.org/licenses/by-nc-sa/3.0/"&gt;</t>
-  </si>
-  <si>
     <t>&lt;mods:abstract&gt;</t>
   </si>
   <si>
@@ -255,7 +252,10 @@
     <t>&lt;mods:physicalDescription displayLabel="Duration"&gt;&lt;mods:extent unit="hours"&gt;</t>
   </si>
   <si>
-    <t>"Creative Commons Attribution-NonCommercial-ShareAlike 3.0 Unported License. You may freely copy, modify, and share these items for non-commercial purposes under the same terms if they include original source information."</t>
+    <t>&lt;mods:accessCondition displayLabel="License" type="use and reproduction" xlink:href="https://creativecommons.org/licenses/by-nc-sa/4.0/"&gt;</t>
+  </si>
+  <si>
+    <t>"Attribution-NonCommercial-ShareAlike 4.0 International (CC BY-NC-SA 4.0)"</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
   <dimension ref="A1:BM1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -745,7 +747,7 @@
         <v>31</v>
       </c>
       <c r="AF1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>2</v>
@@ -790,7 +792,7 @@
         <v>36</v>
       </c>
       <c r="AU1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV1" s="4" t="s">
         <v>9</v>
@@ -799,7 +801,7 @@
         <v>37</v>
       </c>
       <c r="AX1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>12</v>
@@ -826,7 +828,7 @@
         <v>42</v>
       </c>
       <c r="BG1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BH1" s="1" t="s">
         <v>14</v>
@@ -835,7 +837,7 @@
         <v>34</v>
       </c>
       <c r="BJ1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="BK1" s="1" t="s">
         <v>15</v>
@@ -858,7 +860,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SA interviews can have 3 interviewees
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/SA-MODS-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/goslen_ad_unc_edu/Documents/Desktop/update-sa-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96006D6A-0EE2-40AB-9B61-D08C696F0DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{96006D6A-0EE2-40AB-9B61-D08C696F0DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AADAE6D2-0FCD-45B1-AEBB-1F966E4BB486}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="810" windowWidth="25710" windowHeight="13620" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
   <si>
     <t>Contributor (Participant) Name</t>
   </si>
@@ -256,6 +256,60 @@
   </si>
   <si>
     <t>"Attribution-NonCommercial-ShareAlike 4.0 International (CC BY-NC-SA 4.0)"</t>
+  </si>
+  <si>
+    <t>Gender Identity, Sexuality (Contributor 1)</t>
+  </si>
+  <si>
+    <t>Ethnic or Racial Identity (Contributor 1)</t>
+  </si>
+  <si>
+    <t>Pronouns (Contributor 1)</t>
+  </si>
+  <si>
+    <t>Age at recording (Contributor 1)</t>
+  </si>
+  <si>
+    <t>Participant Correct Spelling (Contributor 1)</t>
+  </si>
+  <si>
+    <t>Contributor 1 (Participant) Name</t>
+  </si>
+  <si>
+    <t>Contributor 2 (Participant) Name</t>
+  </si>
+  <si>
+    <t>Gender Identity, Sexuality (Contributor 2)</t>
+  </si>
+  <si>
+    <t>Ethnic or Racial Identity (Contributor 2)</t>
+  </si>
+  <si>
+    <t>Pronouns (Contributor 2)</t>
+  </si>
+  <si>
+    <t>Age at recording (Contributor 2)</t>
+  </si>
+  <si>
+    <t>Participant Correct Spelling (Contributor 2)</t>
+  </si>
+  <si>
+    <t>Contributor 3 (Participant) Name</t>
+  </si>
+  <si>
+    <t>Gender Identity, Sexuality (Contributor 3)</t>
+  </si>
+  <si>
+    <t>Ethnic or Racial Identity (Contributor 3)</t>
+  </si>
+  <si>
+    <t>Pronouns (Contributor 3)</t>
+  </si>
+  <si>
+    <t>Age at recording (Contributor 3)</t>
+  </si>
+  <si>
+    <t>Participant Correct Spelling (Contributor 3)</t>
   </si>
 </sst>
 </file>
@@ -286,12 +340,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,14 +396,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
-  <dimension ref="A1:BM1"/>
+  <dimension ref="A1:CY1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,17 +740,18 @@
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" customWidth="1"/>
     <col min="20" max="20" width="24.85546875" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" customWidth="1"/>
-    <col min="36" max="36" width="17.5703125" customWidth="1"/>
-    <col min="39" max="39" width="30.85546875" customWidth="1"/>
-    <col min="48" max="48" width="9.140625" style="5"/>
-    <col min="51" max="51" width="12.5703125" style="5" customWidth="1"/>
-    <col min="57" max="57" width="18.28515625" customWidth="1"/>
+    <col min="23" max="60" width="9.140625" style="8"/>
+    <col min="62" max="62" width="9.140625" customWidth="1"/>
+    <col min="65" max="65" width="18.5703125" customWidth="1"/>
+    <col min="71" max="71" width="11.28515625" customWidth="1"/>
+    <col min="74" max="74" width="17.5703125" customWidth="1"/>
+    <col min="77" max="77" width="30.85546875" customWidth="1"/>
+    <col min="86" max="86" width="9.140625" style="4"/>
+    <col min="89" max="89" width="12.5703125" style="4" customWidth="1"/>
+    <col min="95" max="95" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -662,190 +761,304 @@
       <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="K1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="N1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="T1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="BD1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BG1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="BH1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="BI1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="BK1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="BL1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="BN1" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="BO1" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BQ1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BR1" t="s">
         <v>68</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="BT1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="BU1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BW1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BX1" t="s">
         <v>45</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BZ1" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="CA1" t="s">
         <v>46</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="CC1" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="CD1" t="s">
         <v>35</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="CF1" t="s">
         <v>36</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="CG1" t="s">
         <v>71</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="CH1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="CI1" t="s">
         <v>37</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="CJ1" t="s">
         <v>70</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="CK1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="CL1" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="CM1" t="s">
         <v>39</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="CO1" t="s">
         <v>40</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="CP1" t="s">
         <v>41</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="CR1" t="s">
         <v>42</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="CS1" t="s">
         <v>69</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="CU1" t="s">
         <v>34</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="CV1" t="s">
         <v>72</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="CX1" t="s">
         <v>43</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="CY1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -877,7 +1090,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
@@ -885,7 +1098,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -893,32 +1106,32 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
@@ -926,7 +1139,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
@@ -934,7 +1147,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
@@ -942,7 +1155,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -950,7 +1163,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
@@ -958,7 +1171,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
       <c r="B14" t="s">
@@ -966,7 +1179,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="B15" t="s">
@@ -974,12 +1187,12 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
@@ -987,7 +1200,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
@@ -995,7 +1208,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
@@ -1003,7 +1216,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
@@ -1011,7 +1224,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
@@ -1019,7 +1232,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">

</xml_diff>